<commit_message>
update calcofi data with correction of vellela lon
</commit_message>
<xml_diff>
--- a/data/20250519_CalCOFI Coding Form (Responses).xlsx
+++ b/data/20250519_CalCOFI Coding Form (Responses).xlsx
@@ -1521,10 +1521,10 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -4187,8 +4187,8 @@
       <c r="R6" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="S6" s="6">
-        <v>-122.561695</v>
+      <c r="S6" s="13">
+        <v>-132.041327</v>
       </c>
       <c r="T6" s="6" t="s">
         <v>247</v>
@@ -4697,22 +4697,22 @@
       <c r="IC7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="13">
+      <c r="A8" s="14">
         <v>45782.52606931713</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>5.0</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4737,22 +4737,22 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <v>45782.54443284722</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>7.0</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4777,58 +4777,58 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13">
+      <c r="A12" s="14">
         <v>45782.56211694445</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>9.0</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>256</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K12" s="14" t="s">
+      <c r="J12" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K12" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="13">
         <v>32.15844</v>
       </c>
-      <c r="Q12" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R12" s="14" t="s">
+      <c r="Q12" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R12" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="S12" s="14">
+      <c r="S12" s="13">
         <v>-117.235761</v>
       </c>
-      <c r="T12" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U12" s="14" t="s">
+      <c r="T12" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U12" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="W12" s="14">
+      <c r="W12" s="13">
         <v>1959.0</v>
       </c>
-      <c r="X12" s="14" t="s">
+      <c r="X12" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -4940,352 +4940,352 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="13">
+      <c r="A14" s="14">
         <v>45784.40906387732</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>11.0</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="J14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K14" s="14" t="s">
+      <c r="J14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="N14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="13">
         <v>32.839</v>
       </c>
-      <c r="Q14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R14" s="14" t="s">
+      <c r="Q14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S14" s="14">
+      <c r="S14" s="13">
         <v>-117.416177</v>
       </c>
-      <c r="T14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U14" s="14" t="s">
+      <c r="T14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="W14" s="14">
+      <c r="W14" s="13">
         <v>1957.0</v>
       </c>
-      <c r="X14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y14" s="14" t="s">
+      <c r="X14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y14" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="Z14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AE14" s="14" t="s">
+      <c r="Z14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE14" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="AF14" s="14" t="s">
+      <c r="AF14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="AG14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AH14" s="14" t="s">
+      <c r="AG14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH14" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AL14" s="14" t="s">
+      <c r="AL14" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="AM14" s="14">
+      <c r="AM14" s="13">
         <v>36.64</v>
       </c>
-      <c r="AN14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="AO14" s="14" t="s">
+      <c r="AN14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="AO14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="AP14" s="14">
+      <c r="AP14" s="13">
         <v>-122.063636</v>
       </c>
-      <c r="AQ14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="AR14" s="14" t="s">
+      <c r="AQ14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="AR14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="AT14" s="14">
+      <c r="AT14" s="13">
         <v>1958.0</v>
       </c>
-      <c r="AU14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AV14" s="14" t="s">
+      <c r="AU14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV14" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="AW14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="BB14" s="14" t="s">
+      <c r="AW14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="BB14" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="BC14" s="14" t="s">
+      <c r="BC14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="BD14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="BE14" s="14" t="s">
+      <c r="BD14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="BE14" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="BI14" s="14" t="s">
+      <c r="BI14" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="BJ14" s="14">
+      <c r="BJ14" s="13">
         <v>32.69</v>
       </c>
-      <c r="BK14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="BL14" s="14" t="s">
+      <c r="BK14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="BL14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="BM14" s="14">
+      <c r="BM14" s="13">
         <v>-117.368929</v>
       </c>
-      <c r="BN14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="BO14" s="14" t="s">
+      <c r="BN14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="BO14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="BP14" s="14" t="s">
+      <c r="BP14" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="BQ14" s="14">
+      <c r="BQ14" s="13">
         <v>1958.0</v>
       </c>
-      <c r="BR14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="BY14" s="14" t="s">
+      <c r="BR14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="BY14" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="BZ14" s="14" t="s">
+      <c r="BZ14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="CA14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="CB14" s="14" t="s">
+      <c r="CA14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CB14" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="CF14" s="14" t="s">
+      <c r="CF14" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="CG14" s="14">
+      <c r="CG14" s="13">
         <v>33.618</v>
       </c>
-      <c r="CH14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="CI14" s="14" t="s">
+      <c r="CH14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="CI14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="CJ14" s="14">
+      <c r="CJ14" s="13">
         <v>-118.400066</v>
       </c>
-      <c r="CK14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="CL14" s="14" t="s">
+      <c r="CK14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="CL14" s="13" t="s">
         <v>248</v>
       </c>
       <c r="CM14" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="CN14" s="14">
+      <c r="CN14" s="13">
         <v>1959.0</v>
       </c>
-      <c r="CO14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="CP14" s="14" t="s">
+      <c r="CO14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="CP14" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="CQ14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="CV14" s="14" t="s">
+      <c r="CQ14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="CV14" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="CW14" s="14" t="s">
+      <c r="CW14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="CX14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="CY14" s="14" t="s">
+      <c r="CX14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CY14" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="DC14" s="14" t="s">
+      <c r="DC14" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="DD14" s="14">
+      <c r="DD14" s="13">
         <v>33.7</v>
       </c>
-      <c r="DE14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="DF14" s="14" t="s">
+      <c r="DE14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="DF14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="DG14" s="14">
+      <c r="DG14" s="13">
         <v>-118.304486</v>
       </c>
-      <c r="DH14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="DI14" s="14" t="s">
+      <c r="DH14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="DI14" s="13" t="s">
         <v>248</v>
       </c>
       <c r="DJ14" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="DK14" s="14">
+      <c r="DK14" s="13">
         <v>1959.0</v>
       </c>
-      <c r="DL14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="DM14" s="14" t="s">
+      <c r="DL14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="DM14" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="DN14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="DS14" s="14" t="s">
+      <c r="DN14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="DS14" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="DT14" s="14" t="s">
+      <c r="DT14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="DU14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="DV14" s="14" t="s">
+      <c r="DU14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="DV14" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="DZ14" s="14" t="s">
+      <c r="DZ14" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="EA14" s="14">
+      <c r="EA14" s="13">
         <v>33.28</v>
       </c>
-      <c r="EB14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="EC14" s="14" t="s">
+      <c r="EB14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="EC14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="ED14" s="14">
+      <c r="ED14" s="13">
         <v>-119.556245</v>
       </c>
-      <c r="EE14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="EF14" s="14" t="s">
+      <c r="EE14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="EF14" s="13" t="s">
         <v>248</v>
       </c>
       <c r="EG14" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="EH14" s="14">
+      <c r="EH14" s="13">
         <v>1959.0</v>
       </c>
-      <c r="EI14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="EJ14" s="14" t="s">
+      <c r="EI14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="EJ14" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="EK14" s="14" t="s">
+      <c r="EK14" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="EP14" s="14" t="s">
+      <c r="EP14" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="EQ14" s="14" t="s">
+      <c r="EQ14" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="ER14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="ES14" s="14" t="s">
+      <c r="ER14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="ES14" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="EW14" s="14" t="s">
+      <c r="EW14" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="EX14" s="14">
+      <c r="EX14" s="13">
         <v>33.384</v>
       </c>
-      <c r="EY14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="EZ14" s="14" t="s">
+      <c r="EY14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="EZ14" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="FA14" s="14">
+      <c r="FA14" s="13">
         <v>-118.492346</v>
       </c>
-      <c r="FB14" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="FC14" s="14" t="s">
+      <c r="FB14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="FC14" s="13" t="s">
         <v>248</v>
       </c>
       <c r="FD14" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="FE14" s="14">
+      <c r="FE14" s="13">
         <v>1960.0</v>
       </c>
-      <c r="FF14" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="FG14" s="14" t="s">
+      <c r="FF14" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="FG14" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="FH14" s="14" t="s">
+      <c r="FH14" s="13" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5355,22 +5355,22 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="14">
         <v>45784.42070315972</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>13.0</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>240</v>
       </c>
       <c r="IC16" s="19" t="s">
@@ -5401,19 +5401,19 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="13">
+      <c r="A18" s="14">
         <v>45784.43606046296</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>15.0</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>239</v>
       </c>
       <c r="F18" s="20" t="s">
@@ -5489,22 +5489,22 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="13">
+      <c r="A20" s="14">
         <v>45784.457042650465</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="13">
         <v>17.0</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -5532,67 +5532,67 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="13">
+      <c r="A22" s="14">
         <v>45784.476067615746</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <v>19.0</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="J22" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K22" s="14" t="s">
+      <c r="J22" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K22" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O22" s="14" t="s">
+      <c r="O22" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="P22" s="14">
+      <c r="P22" s="13">
         <v>34.43</v>
       </c>
-      <c r="Q22" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R22" s="14" t="s">
+      <c r="Q22" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R22" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S22" s="14">
+      <c r="S22" s="13">
         <v>-120.517286</v>
       </c>
-      <c r="T22" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U22" s="14" t="s">
+      <c r="T22" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U22" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V22" s="14" t="s">
+      <c r="V22" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="W22" s="14">
+      <c r="W22" s="13">
         <v>1975.0</v>
       </c>
-      <c r="X22" s="14" t="s">
+      <c r="X22" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="Y22" s="14" t="s">
+      <c r="Y22" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="Z22" s="14" t="s">
+      <c r="Z22" s="13" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5671,22 +5671,22 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13">
+      <c r="A24" s="14">
         <v>45784.49582469907</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="13">
         <v>21.0</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>303</v>
       </c>
       <c r="IC24" s="19" t="s">
@@ -5714,118 +5714,118 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13">
+      <c r="A26" s="14">
         <v>45784.77504439815</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="13">
         <v>23.0</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="13" t="s">
         <v>306</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K26" s="14" t="s">
+      <c r="J26" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K26" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O26" s="14" t="s">
+      <c r="O26" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26" s="13">
         <v>32.77</v>
       </c>
-      <c r="Q26" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R26" s="14" t="s">
+      <c r="Q26" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R26" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S26" s="14">
+      <c r="S26" s="13">
         <v>-117.348996</v>
       </c>
-      <c r="T26" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U26" s="14" t="s">
+      <c r="T26" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U26" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V26" s="14" t="s">
+      <c r="V26" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W26" s="14">
+      <c r="W26" s="13">
         <v>1978.0</v>
       </c>
-      <c r="X26" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y26" s="14" t="s">
+      <c r="X26" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y26" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="Z26" s="14" t="s">
+      <c r="Z26" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AE26" s="14" t="s">
+      <c r="AE26" s="13" t="s">
         <v>266</v>
       </c>
       <c r="AF26" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="AG26" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AH26" s="14" t="s">
+      <c r="AG26" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH26" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AL26" s="14" t="s">
+      <c r="AL26" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="AM26" s="14">
+      <c r="AM26" s="13">
         <v>36.52</v>
       </c>
-      <c r="AN26" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="AO26" s="14" t="s">
+      <c r="AN26" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="AO26" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="AP26" s="14">
+      <c r="AP26" s="13">
         <v>-122.084259</v>
       </c>
-      <c r="AQ26" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="AR26" s="14" t="s">
+      <c r="AQ26" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="AR26" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="AS26" s="14" t="s">
+      <c r="AS26" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="AT26" s="14">
+      <c r="AT26" s="13">
         <v>1978.0</v>
       </c>
-      <c r="AU26" s="14" t="s">
+      <c r="AU26" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AV26" s="14" t="s">
+      <c r="AV26" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="AW26" s="14" t="s">
+      <c r="AW26" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AZ26" s="14" t="s">
+      <c r="AZ26" s="13" t="s">
         <v>311</v>
       </c>
     </row>
@@ -5850,76 +5850,76 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13">
+      <c r="A28" s="14">
         <v>45788.58684625</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="13">
         <v>69.0</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K28" s="14" t="s">
+      <c r="J28" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K28" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O28" s="14" t="s">
+      <c r="O28" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="P28" s="14">
+      <c r="P28" s="13">
         <v>34.4208</v>
       </c>
-      <c r="Q28" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R28" s="14" t="s">
+      <c r="Q28" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R28" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="S28" s="14">
+      <c r="S28" s="13">
         <v>-119.7</v>
       </c>
-      <c r="T28" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U28" s="14" t="s">
+      <c r="T28" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U28" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="V28" s="14" t="s">
+      <c r="V28" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="W28" s="14">
+      <c r="W28" s="13">
         <v>1958.0</v>
       </c>
-      <c r="X28" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y28" s="14" t="s">
+      <c r="X28" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y28" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="Z28" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA28" s="14">
+      <c r="Z28" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA28" s="13">
         <v>24.0</v>
       </c>
-      <c r="AB28" s="14" t="s">
+      <c r="AB28" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AC28" s="14" t="s">
+      <c r="AC28" s="13" t="s">
         <v>318</v>
       </c>
       <c r="IC28" s="19" t="s">
@@ -5947,22 +5947,22 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="13">
+      <c r="A30" s="14">
         <v>45789.39098454861</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <v>26.0</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="13" t="s">
         <v>240</v>
       </c>
       <c r="IC30" s="19" t="s">
@@ -6056,25 +6056,25 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="13">
+      <c r="A32" s="14">
         <v>45789.41318902778</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="13">
         <v>27.0</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="L32" s="13" t="s">
         <v>257</v>
       </c>
     </row>
@@ -6099,61 +6099,61 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="13">
+      <c r="A34" s="14">
         <v>45789.42182721065</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="13">
         <v>29.0</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J34" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K34" s="14" t="s">
+      <c r="J34" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K34" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O34" s="14" t="s">
+      <c r="O34" s="13" t="s">
         <v>326</v>
       </c>
-      <c r="P34" s="14">
+      <c r="P34" s="13">
         <v>33.566</v>
       </c>
-      <c r="Q34" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R34" s="14" t="s">
+      <c r="Q34" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R34" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S34" s="14">
+      <c r="S34" s="13">
         <v>-118.884083</v>
       </c>
-      <c r="T34" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U34" s="14" t="s">
+      <c r="T34" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U34" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V34" s="14" t="s">
+      <c r="V34" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="W34" s="14">
+      <c r="W34" s="13">
         <v>1983.0</v>
       </c>
-      <c r="X34" s="14" t="s">
+      <c r="X34" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -6445,22 +6445,22 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="13">
+      <c r="A36" s="14">
         <v>45789.45341189815</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D36" s="14">
+      <c r="D36" s="13">
         <v>31.0</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="13" t="s">
         <v>303</v>
       </c>
     </row>
@@ -6485,22 +6485,22 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="13">
+      <c r="A38" s="14">
         <v>45789.47250240741</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="13">
         <v>33.0</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6573,127 +6573,127 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="13">
+      <c r="A40" s="14">
         <v>45789.50098138889</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="13">
         <v>35.0</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="H40" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="K40" s="14" t="s">
+      <c r="K40" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O40" s="14" t="s">
+      <c r="O40" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="P40" s="14">
+      <c r="P40" s="13">
         <v>33.65</v>
       </c>
-      <c r="Q40" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="R40" s="14" t="s">
+      <c r="Q40" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="R40" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="S40" s="14">
+      <c r="S40" s="13">
         <v>-118.97</v>
       </c>
-      <c r="T40" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="U40" s="14" t="s">
+      <c r="T40" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="U40" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="V40" s="14" t="s">
+      <c r="V40" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="W40" s="14">
+      <c r="W40" s="13">
         <v>1984.0</v>
       </c>
-      <c r="X40" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y40" s="14" t="s">
+      <c r="X40" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y40" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="Z40" s="14" t="s">
+      <c r="Z40" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AA40" s="14">
+      <c r="AA40" s="13">
         <v>31.0</v>
       </c>
-      <c r="AB40" s="14" t="s">
+      <c r="AB40" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AE40" s="14" t="s">
+      <c r="AE40" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="AF40" s="14" t="s">
+      <c r="AF40" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="AG40" s="14" t="s">
+      <c r="AG40" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="AH40" s="14" t="s">
+      <c r="AH40" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AL40" s="14" t="s">
+      <c r="AL40" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="AM40" s="14">
+      <c r="AM40" s="13">
         <v>36.182</v>
       </c>
-      <c r="AN40" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AO40" s="14" t="s">
+      <c r="AN40" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO40" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="AP40" s="14">
+      <c r="AP40" s="13">
         <v>-122.77</v>
       </c>
-      <c r="AQ40" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AR40" s="14" t="s">
+      <c r="AQ40" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AR40" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="AS40" s="14" t="s">
+      <c r="AS40" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="AT40" s="14">
+      <c r="AT40" s="13">
         <v>1984.0</v>
       </c>
-      <c r="AU40" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AV40" s="14" t="s">
+      <c r="AU40" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV40" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="AW40" s="14" t="s">
+      <c r="AW40" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AX40" s="14">
+      <c r="AX40" s="13">
         <v>31.0</v>
       </c>
-      <c r="AY40" s="14" t="s">
+      <c r="AY40" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -6718,70 +6718,70 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="13">
+      <c r="A42" s="14">
         <v>45789.50648740741</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D42" s="13">
         <v>37.0</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="I42" s="14" t="s">
+      <c r="I42" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="J42" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K42" s="14" t="s">
+      <c r="J42" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K42" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="L42" s="14" t="s">
+      <c r="L42" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="M42" s="14" t="s">
+      <c r="M42" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="N42" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="O42" s="14" t="s">
+      <c r="N42" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="O42" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="P42" s="14">
+      <c r="P42" s="13">
         <v>32.93</v>
       </c>
-      <c r="Q42" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R42" s="14" t="s">
+      <c r="Q42" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R42" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S42" s="14">
+      <c r="S42" s="13">
         <v>-118.490725</v>
       </c>
-      <c r="T42" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U42" s="14" t="s">
+      <c r="T42" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U42" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V42" s="14" t="s">
+      <c r="V42" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="W42" s="14">
+      <c r="W42" s="13">
         <v>1995.0</v>
       </c>
-      <c r="X42" s="14" t="s">
+      <c r="X42" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -6806,67 +6806,67 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="13">
+      <c r="A44" s="14">
         <v>45789.518718101855</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="13">
         <v>39.0</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H44" s="14" t="s">
+      <c r="H44" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="I44" s="14" t="s">
+      <c r="I44" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J44" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K44" s="14" t="s">
+      <c r="J44" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K44" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O44" s="14" t="s">
+      <c r="O44" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="P44" s="14">
+      <c r="P44" s="13">
         <v>32.513</v>
       </c>
-      <c r="Q44" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="R44" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="S44" s="14">
+      <c r="Q44" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="R44" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="S44" s="13">
         <v>-118.21</v>
       </c>
-      <c r="T44" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="U44" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="V44" s="14" t="s">
+      <c r="T44" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="U44" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="V44" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="W44" s="14">
+      <c r="W44" s="13">
         <v>1998.0</v>
       </c>
-      <c r="X44" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y44" s="14" t="s">
+      <c r="X44" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y44" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="Z44" s="14" t="s">
+      <c r="Z44" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -6891,61 +6891,61 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="13">
+      <c r="A46" s="14">
         <v>45789.552373645834</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="13">
         <v>41.0</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H46" s="14" t="s">
+      <c r="H46" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="I46" s="14" t="s">
+      <c r="I46" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J46" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K46" s="14" t="s">
+      <c r="J46" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K46" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="O46" s="14" t="s">
+      <c r="O46" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="P46" s="14">
+      <c r="P46" s="13">
         <v>48.59</v>
       </c>
-      <c r="Q46" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R46" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="S46" s="14">
+      <c r="Q46" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R46" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="S46" s="13">
         <v>-124.990973</v>
       </c>
-      <c r="T46" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U46" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="V46" s="14" t="s">
+      <c r="T46" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U46" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="V46" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="W46" s="14">
+      <c r="W46" s="13">
         <v>1926.0</v>
       </c>
-      <c r="X46" s="14" t="s">
+      <c r="X46" s="13" t="s">
         <v>249</v>
       </c>
     </row>
@@ -7024,22 +7024,22 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="13">
+      <c r="A48" s="14">
         <v>45789.560899398144</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="13">
         <v>43.0</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="13" t="s">
         <v>303</v>
       </c>
     </row>
@@ -7064,115 +7064,115 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="13">
+      <c r="A50" s="14">
         <v>45791.37654513889</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50" s="13">
         <v>45.0</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H50" s="14" t="s">
+      <c r="H50" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="I50" s="14" t="s">
+      <c r="I50" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J50" s="14" t="s">
+      <c r="J50" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="K50" s="14" t="s">
+      <c r="K50" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O50" s="14" t="s">
+      <c r="O50" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="P50" s="14">
+      <c r="P50" s="13">
         <v>44.65</v>
       </c>
-      <c r="Q50" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="R50" s="14" t="s">
+      <c r="Q50" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="R50" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S50" s="14">
+      <c r="S50" s="13">
         <v>-124.18</v>
       </c>
-      <c r="T50" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="U50" s="14" t="s">
+      <c r="T50" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="U50" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V50" s="14" t="s">
+      <c r="V50" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="W50" s="14">
+      <c r="W50" s="13">
         <v>2010.0</v>
       </c>
-      <c r="X50" s="14" t="s">
+      <c r="X50" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="Y50" s="14" t="s">
+      <c r="Y50" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="Z50" s="14" t="s">
+      <c r="Z50" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AE50" s="14" t="s">
+      <c r="AE50" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="AF50" s="14" t="s">
+      <c r="AF50" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="AG50" s="14" t="s">
+      <c r="AG50" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="AH50" s="14" t="s">
+      <c r="AH50" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AL50" s="14" t="s">
+      <c r="AL50" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="AM50" s="14">
+      <c r="AM50" s="13">
         <v>44.65</v>
       </c>
-      <c r="AN50" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AO50" s="14" t="s">
+      <c r="AN50" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO50" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="AP50" s="14">
+      <c r="AP50" s="13">
         <v>-124.18</v>
       </c>
-      <c r="AQ50" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AR50" s="14" t="s">
+      <c r="AQ50" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AR50" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="AS50" s="14" t="s">
+      <c r="AS50" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="AT50" s="14">
+      <c r="AT50" s="13">
         <v>2010.0</v>
       </c>
-      <c r="AU50" s="14" t="s">
+      <c r="AU50" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AV50" s="14" t="s">
+      <c r="AV50" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="AW50" s="14" t="s">
+      <c r="AW50" s="13" t="s">
         <v>265</v>
       </c>
       <c r="IC50" s="19" t="s">
@@ -7251,82 +7251,82 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="13">
+      <c r="A52" s="14">
         <v>45791.412773495365</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D52" s="14">
+      <c r="D52" s="13">
         <v>47.0</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="I52" s="14" t="s">
+      <c r="I52" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J52" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K52" s="14" t="s">
+      <c r="J52" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K52" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="L52" s="14" t="s">
+      <c r="L52" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="M52" s="14" t="s">
+      <c r="M52" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="N52" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="O52" s="14" t="s">
+      <c r="N52" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="O52" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="P52" s="14">
+      <c r="P52" s="13">
         <v>44.0</v>
       </c>
-      <c r="Q52" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="R52" s="14" t="s">
+      <c r="Q52" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="R52" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="S52" s="14">
+      <c r="S52" s="13">
         <v>-124.286333</v>
       </c>
-      <c r="T52" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U52" s="14" t="s">
+      <c r="T52" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U52" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="V52" s="14" t="s">
+      <c r="V52" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="W52" s="14">
+      <c r="W52" s="13">
         <v>2009.0</v>
       </c>
-      <c r="X52" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y52" s="14" t="s">
+      <c r="X52" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y52" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="Z52" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA52" s="14">
+      <c r="Z52" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA52" s="13">
         <v>18.0</v>
       </c>
-      <c r="AC52" s="14" t="s">
+      <c r="AC52" s="13" t="s">
         <v>365</v>
       </c>
     </row>
@@ -7351,79 +7351,79 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="13">
+      <c r="A54" s="14">
         <v>45791.432106504624</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="13">
         <v>49.0</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="H54" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="I54" s="14" t="s">
+      <c r="I54" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J54" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K54" s="14" t="s">
+      <c r="J54" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K54" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="L54" s="14" t="s">
+      <c r="L54" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="M54" s="14" t="s">
+      <c r="M54" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="N54" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="O54" s="14" t="s">
+      <c r="N54" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="O54" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="P54" s="14">
+      <c r="P54" s="13">
         <v>34.89</v>
       </c>
-      <c r="Q54" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="R54" s="14" t="s">
+      <c r="Q54" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="R54" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="S54" s="14">
+      <c r="S54" s="13">
         <v>-121.19831</v>
       </c>
-      <c r="T54" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="U54" s="14" t="s">
+      <c r="T54" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="U54" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="V54" s="14" t="s">
+      <c r="V54" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="W54" s="14">
+      <c r="W54" s="13">
         <v>2008.0</v>
       </c>
-      <c r="X54" s="14" t="s">
+      <c r="X54" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="Y54" s="14" t="s">
+      <c r="Y54" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="Z54" s="14" t="s">
+      <c r="Z54" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AC54" s="14" t="s">
+      <c r="AC54" s="13" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7502,307 +7502,307 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="13">
+      <c r="A56" s="14">
         <v>45791.46713900463</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D56" s="14">
+      <c r="D56" s="13">
         <v>51.0</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H56" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="I56" s="14" t="s">
+      <c r="I56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K56" s="14" t="s">
+      <c r="J56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K56" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="L56" s="14" t="s">
+      <c r="L56" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="M56" s="14" t="s">
+      <c r="M56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="N56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="O56" s="14" t="s">
+      <c r="N56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="O56" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="P56" s="14">
+      <c r="P56" s="13">
         <v>36.0</v>
       </c>
-      <c r="Q56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="R56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="S56" s="14">
+      <c r="Q56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="R56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="S56" s="13">
         <v>-121.6</v>
       </c>
-      <c r="T56" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="V56" s="14" t="s">
+      <c r="T56" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="V56" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="W56" s="14">
+      <c r="W56" s="13">
         <v>2015.0</v>
       </c>
-      <c r="X56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y56" s="14" t="s">
+      <c r="X56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y56" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="Z56" s="14" t="s">
+      <c r="Z56" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AE56" s="14" t="s">
+      <c r="AE56" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="AF56" s="14" t="s">
+      <c r="AF56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="AG56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AH56" s="14" t="s">
+      <c r="AG56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH56" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AI56" s="14" t="s">
+      <c r="AI56" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="AJ56" s="14" t="s">
+      <c r="AJ56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="AK56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AL56" s="14" t="s">
+      <c r="AK56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL56" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="AM56" s="14">
+      <c r="AM56" s="13">
         <v>36.0</v>
       </c>
-      <c r="AN56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AO56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AP56" s="14">
+      <c r="AN56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AP56" s="13">
         <v>-121.6</v>
       </c>
-      <c r="AQ56" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="AR56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AS56" s="14" t="s">
+      <c r="AQ56" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="AR56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AS56" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="AT56" s="14">
+      <c r="AT56" s="13">
         <v>2015.0</v>
       </c>
-      <c r="AU56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AV56" s="14" t="s">
+      <c r="AU56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV56" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="AW56" s="14" t="s">
+      <c r="AW56" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AZ56" s="14" t="s">
+      <c r="AZ56" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="BB56" s="14" t="s">
+      <c r="BB56" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="BC56" s="14" t="s">
+      <c r="BC56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="BD56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="BE56" s="14" t="s">
+      <c r="BD56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="BE56" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="BF56" s="14" t="s">
+      <c r="BF56" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="BG56" s="14" t="s">
+      <c r="BG56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="BH56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="BI56" s="14" t="s">
+      <c r="BH56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="BI56" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="BJ56" s="14">
+      <c r="BJ56" s="13">
         <v>36.0</v>
       </c>
-      <c r="BK56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="BL56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="BM56" s="14">
+      <c r="BK56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="BL56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="BM56" s="13">
         <v>-121.6</v>
       </c>
-      <c r="BN56" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="BO56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="BP56" s="14" t="s">
+      <c r="BN56" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="BO56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="BP56" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="BQ56" s="14">
+      <c r="BQ56" s="13">
         <v>2015.0</v>
       </c>
-      <c r="BR56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="BS56" s="14" t="s">
+      <c r="BR56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="BS56" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="BT56" s="14" t="s">
+      <c r="BT56" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="BY56" s="14" t="s">
+      <c r="BY56" s="13" t="s">
         <v>378</v>
       </c>
-      <c r="BZ56" s="14" t="s">
+      <c r="BZ56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="CA56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="CB56" s="14" t="s">
+      <c r="CA56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CB56" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="CC56" s="14" t="s">
+      <c r="CC56" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="CD56" s="14" t="s">
+      <c r="CD56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="CE56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="CF56" s="14" t="s">
+      <c r="CE56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CF56" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="CG56" s="14">
+      <c r="CG56" s="13">
         <v>36.0</v>
       </c>
-      <c r="CH56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="CI56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="CJ56" s="14">
+      <c r="CH56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="CI56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CJ56" s="13">
         <v>-121.6</v>
       </c>
-      <c r="CK56" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="CL56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="CM56" s="14" t="s">
+      <c r="CK56" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="CL56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CM56" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="CN56" s="14">
+      <c r="CN56" s="13">
         <v>2015.0</v>
       </c>
-      <c r="CO56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="CP56" s="14" t="s">
+      <c r="CO56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="CP56" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="CQ56" s="14" t="s">
+      <c r="CQ56" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="CV56" s="14" t="s">
+      <c r="CV56" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="CW56" s="14" t="s">
+      <c r="CW56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="CX56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="CY56" s="14" t="s">
+      <c r="CX56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CY56" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="CZ56" s="14" t="s">
+      <c r="CZ56" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="DA56" s="14" t="s">
+      <c r="DA56" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="DB56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="DC56" s="14" t="s">
+      <c r="DB56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="DC56" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="DD56" s="14">
+      <c r="DD56" s="13">
         <v>36.0</v>
       </c>
-      <c r="DE56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="DF56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="DG56" s="14">
+      <c r="DE56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="DF56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="DG56" s="13">
         <v>-121.6</v>
       </c>
-      <c r="DH56" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="DI56" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="DJ56" s="14" t="s">
+      <c r="DH56" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="DI56" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="DJ56" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="DK56" s="14">
+      <c r="DK56" s="13">
         <v>2015.0</v>
       </c>
-      <c r="DL56" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="DM56" s="14" t="s">
+      <c r="DL56" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="DM56" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="DN56" s="14" t="s">
+      <c r="DN56" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -7881,76 +7881,76 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="13">
+      <c r="A58" s="14">
         <v>45791.837182337964</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D58" s="14">
+      <c r="D58" s="13">
         <v>53.0</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="H58" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="I58" s="14" t="s">
+      <c r="I58" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J58" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K58" s="14" t="s">
+      <c r="J58" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K58" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="L58" s="14" t="s">
+      <c r="L58" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="M58" s="14" t="s">
+      <c r="M58" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="N58" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="O58" s="14" t="s">
+      <c r="N58" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="O58" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="P58" s="14">
+      <c r="P58" s="13">
         <v>32.539285</v>
       </c>
-      <c r="Q58" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R58" s="14" t="s">
+      <c r="Q58" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R58" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S58" s="14">
+      <c r="S58" s="13">
         <v>-117.129169</v>
       </c>
-      <c r="T58" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U58" s="14" t="s">
+      <c r="T58" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U58" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V58" s="14" t="s">
+      <c r="V58" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="W58" s="14">
+      <c r="W58" s="13">
         <v>2015.0</v>
       </c>
-      <c r="X58" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y58" s="14" t="s">
+      <c r="X58" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y58" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="Z58" s="14" t="s">
+      <c r="Z58" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -8035,79 +8035,79 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="13">
+      <c r="A60" s="14">
         <v>45792.35618832176</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D60" s="14">
+      <c r="D60" s="13">
         <v>55.0</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H60" s="14" t="s">
+      <c r="H60" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="I60" s="14" t="s">
+      <c r="I60" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J60" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K60" s="14" t="s">
+      <c r="J60" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K60" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="L60" s="14" t="s">
+      <c r="L60" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="M60" s="14" t="s">
+      <c r="M60" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="N60" s="14" t="s">
+      <c r="N60" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="O60" s="14" t="s">
+      <c r="O60" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="P60" s="14">
+      <c r="P60" s="13">
         <v>37.76687</v>
       </c>
-      <c r="Q60" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R60" s="14" t="s">
+      <c r="Q60" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R60" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="S60" s="14">
+      <c r="S60" s="13">
         <v>-123.08237</v>
       </c>
-      <c r="T60" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U60" s="14" t="s">
+      <c r="T60" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U60" s="13" t="s">
         <v>248</v>
       </c>
       <c r="V60" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="W60" s="14">
+      <c r="W60" s="13">
         <v>2015.0</v>
       </c>
-      <c r="X60" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y60" s="14" t="s">
+      <c r="X60" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y60" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="Z60" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AC60" s="14" t="s">
+      <c r="Z60" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC60" s="13" t="s">
         <v>391</v>
       </c>
     </row>
@@ -8132,22 +8132,22 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="13">
+      <c r="A62" s="14">
         <v>45793.583910497684</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D62" s="14">
+      <c r="D62" s="13">
         <v>57.0</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F62" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -8172,22 +8172,22 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="13">
+      <c r="A64" s="14">
         <v>45793.58569091435</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D64" s="14">
+      <c r="D64" s="13">
         <v>59.0</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F64" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -8314,22 +8314,22 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="13">
+      <c r="A66" s="14">
         <v>45796.36752722222</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D66" s="14">
+      <c r="D66" s="13">
         <v>61.0</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="F66" s="14" t="s">
+      <c r="F66" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -8420,127 +8420,127 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="13">
+      <c r="A68" s="14">
         <v>45796.38891858797</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D68" s="14">
+      <c r="D68" s="13">
         <v>63.0</v>
       </c>
-      <c r="E68" s="14" t="s">
+      <c r="E68" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H68" s="14" t="s">
+      <c r="H68" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="I68" s="14" t="s">
+      <c r="I68" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J68" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K68" s="14" t="s">
+      <c r="J68" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K68" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O68" s="14" t="s">
+      <c r="O68" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="P68" s="14">
+      <c r="P68" s="13">
         <v>36.35</v>
       </c>
-      <c r="Q68" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="R68" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="S68" s="14">
+      <c r="Q68" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="R68" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="S68" s="13">
         <v>-121.9807</v>
       </c>
-      <c r="T68" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U68" s="14" t="s">
+      <c r="T68" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U68" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V68" s="14" t="s">
+      <c r="V68" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="W68" s="14">
+      <c r="W68" s="13">
         <v>2015.0</v>
       </c>
-      <c r="X68" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y68" s="14" t="s">
+      <c r="X68" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y68" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="Z68" s="14" t="s">
+      <c r="Z68" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AC68" s="14" t="s">
+      <c r="AC68" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="AE68" s="14" t="s">
+      <c r="AE68" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="AF68" s="14" t="s">
+      <c r="AF68" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="AG68" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AH68" s="14" t="s">
+      <c r="AG68" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH68" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AI68" s="14" t="s">
+      <c r="AI68" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="AJ68" s="14" t="s">
+      <c r="AJ68" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="AK68" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AL68" s="14" t="s">
+      <c r="AK68" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL68" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="AM68" s="14">
+      <c r="AM68" s="13">
         <v>36.35</v>
       </c>
-      <c r="AN68" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AO68" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AP68" s="14">
+      <c r="AN68" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO68" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AP68" s="13">
         <v>-121.9807</v>
       </c>
-      <c r="AQ68" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="AR68" s="14" t="s">
+      <c r="AQ68" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="AR68" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="AS68" s="14" t="s">
+      <c r="AS68" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="AT68" s="14">
+      <c r="AT68" s="13">
         <v>2015.0</v>
       </c>
-      <c r="AU68" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AV68" s="14" t="s">
+      <c r="AU68" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV68" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="AW68" s="14" t="s">
+      <c r="AW68" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -8664,115 +8664,115 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="13">
+      <c r="A70" s="14">
         <v>45796.4133958912</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D70" s="14">
+      <c r="D70" s="13">
         <v>65.0</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E70" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H70" s="14" t="s">
+      <c r="H70" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="I70" s="14" t="s">
+      <c r="I70" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="J70" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="K70" s="14" t="s">
+      <c r="J70" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K70" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="O70" s="14" t="s">
+      <c r="O70" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="P70" s="14">
+      <c r="P70" s="13">
         <v>41.0</v>
       </c>
-      <c r="Q70" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="R70" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="S70" s="14">
+      <c r="Q70" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="R70" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="S70" s="13">
         <v>-124.26</v>
       </c>
-      <c r="T70" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="U70" s="14" t="s">
+      <c r="T70" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="U70" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="V70" s="14" t="s">
+      <c r="V70" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="W70" s="14">
+      <c r="W70" s="13">
         <v>2019.0</v>
       </c>
-      <c r="X70" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y70" s="14" t="s">
+      <c r="X70" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y70" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="Z70" s="14" t="s">
+      <c r="Z70" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AE70" s="14" t="s">
+      <c r="AE70" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="AF70" s="14" t="s">
+      <c r="AF70" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="AG70" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AH70" s="14" t="s">
+      <c r="AG70" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH70" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AL70" s="14" t="s">
+      <c r="AL70" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="AM70" s="14">
+      <c r="AM70" s="13">
         <v>41.0</v>
       </c>
-      <c r="AN70" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AO70" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AP70" s="14">
+      <c r="AN70" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO70" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="AP70" s="13">
         <v>-124.26</v>
       </c>
-      <c r="AQ70" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="AR70" s="14" t="s">
+      <c r="AQ70" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="AR70" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="AS70" s="14" t="s">
+      <c r="AS70" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="AT70" s="14">
+      <c r="AT70" s="13">
         <v>2019.0</v>
       </c>
-      <c r="AU70" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AV70" s="14" t="s">
+      <c r="AU70" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV70" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="AW70" s="14" t="s">
+      <c r="AW70" s="13" t="s">
         <v>265</v>
       </c>
     </row>

</xml_diff>